<commit_message>
Update artifact import template and processing to match cataloging system
Update artifact import template and processing logic in routes.py to reflect the fields used in the LAARI cataloging system, including adding explanatory text about image handling and updating preview templates.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 91bfc21d-135f-4f37-bb75-e9b5d890c340
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: f0a46eb6-e1dd-48e3-b079-4247b7102f42
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/86f88c59-1b27-4410-98b4-2d7b6d49d99b/91bfc21d-135f-4f37-bb75-e9b5d890c340/JEI2CvT
</commit_message>
<xml_diff>
--- a/static/templates/modelo_importacao_laari.xlsx
+++ b/static/templates/modelo_importacao_laari.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,141 +443,126 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="18" customWidth="1" min="9" max="9"/>
-    <col width="18" customWidth="1" min="10" max="10"/>
-    <col width="18" customWidth="1" min="11" max="11"/>
-    <col width="18" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>codigo</t>
+          <t>nome_artefato</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>nome</t>
+          <t>codigo_artefato</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>tipo_artefato</t>
+          <t>data_descoberta</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>material</t>
+          <t>tipo</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>periodo</t>
+          <t>local_origem</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>cultura</t>
+          <t>localizacao_arqueologica</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>localizacao</t>
+          <t>profundidade</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>descricao</t>
+          <t>nivel_estratigrafico</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>coordenadas</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>estado_conservacao</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>dimensoes</t>
-        </is>
-      </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>data_catalogacao</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>responsavel</t>
+          <t>observacoes</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>ART-001</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Vaso Cerâmico</t>
-        </is>
-      </c>
+          <t>Vaso Cerâmico Tupi</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr"/>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>vaso</t>
+          <t>2024-01-15</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>cerâmica</t>
+          <t>vaso cerâmico</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Pré-colonial</t>
+          <t>Sítio Arqueológico Exemplo, SP</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>Tupi-Guarani</t>
+          <t>Setor A, Quadra 5</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Sítio Exemplo, SP</t>
+          <t>1.20m</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>Vaso de borda reforçada com decoração pintada</t>
+          <t>Nível 3</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>fragmentado</t>
+          <t>-23.5505, -46.6333</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>15cm x 12cm x 10cm</t>
+          <t>bom</t>
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
         <is>
-          <t>2024-01-15</t>
-        </is>
-      </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>Dr. João Silva</t>
+          <t>Fragmento de borda com decoração pintada</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the spreadsheet template to remove example data
Remove all example data from the spreadsheet template, leaving only column headers.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 91bfc21d-135f-4f37-bb75-e9b5d890c340
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: f1221be5-8677-4465-bf29-40784dc7cc3f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/86f88c59-1b27-4410-98b4-2d7b6d49d99b/91bfc21d-135f-4f37-bb75-e9b5d890c340/JEI2CvT
</commit_message>
<xml_diff>
--- a/static/templates/modelo_importacao_laari.xlsx
+++ b/static/templates/modelo_importacao_laari.xlsx
@@ -62,13 +62,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,17 +440,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="22" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="9" max="9"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -510,59 +507,6 @@
       <c r="K1" s="1" t="inlineStr">
         <is>
           <t>observacoes</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>Vaso Cerâmico Tupi</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr"/>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>2024-01-15</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>vaso cerâmico</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>Sítio Arqueológico Exemplo, SP</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>Setor A, Quadra 5</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>1.20m</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>Nível 3</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>-23.5505, -46.6333</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>bom</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>Fragmento de borda com decoração pintada</t>
         </is>
       </c>
     </row>

</xml_diff>